<commit_message>
Atualização de tabela de correlação
</commit_message>
<xml_diff>
--- a/dados/Correlação SCN PIMPF FUNCEX.xlsx
+++ b/dados/Correlação SCN PIMPF FUNCEX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amilton.lobo.MDIC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E15B6400-B207-4409-BEC1-93EDFFF9B63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB170A6-6F6D-4EA6-8D59-B7F68FAEA1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC529E8-EB9C-47CB-ACBC-CD5C4D5BC077}"/>
+    <workbookView xWindow="-16305" yWindow="0" windowWidth="16410" windowHeight="14145" xr2:uid="{ACC529E8-EB9C-47CB-ACBC-CD5C4D5BC077}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>PIM-PF</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>3.10 Fabricação de produtos alimentícios</t>
+  </si>
+  <si>
+    <t>Prefixo Cód. SCN</t>
   </si>
 </sst>
 </file>
@@ -551,207 +554,280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6650BCE3-9743-4CB1-AE40-634175843485}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>31801</v>
+      </c>
+      <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>31802</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -761,6 +837,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b2c27b32-fdd2-4db9-b23b-7ec32a91d3be" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007D5D409EC24D334B996C1CFFCF1C5F5F" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c7ae6990cfdbbe9a7f7b92e321cdfc8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="650c6c8f-6c2a-41c5-9e0c-9cf06d8ec2d7" xmlns:ns4="b2c27b32-fdd2-4db9-b23b-7ec32a91d3be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="237a74c5217cd1015985379078b0dd77" ns3:_="" ns4:_="">
     <xsd:import namespace="650c6c8f-6c2a-41c5-9e0c-9cf06d8ec2d7"/>
@@ -1007,24 +1100,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB14859-9444-49E4-935A-89923E9FF272}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b2c27b32-fdd2-4db9-b23b-7ec32a91d3be"/>
+    <ds:schemaRef ds:uri="650c6c8f-6c2a-41c5-9e0c-9cf06d8ec2d7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b2c27b32-fdd2-4db9-b23b-7ec32a91d3be" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC214C3-9795-4B05-9630-C4DEF512618F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2044316B-E7C0-4893-B9F9-CB2CF15ADD1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1041,29 +1142,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC214C3-9795-4B05-9630-C4DEF512618F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB14859-9444-49E4-935A-89923E9FF272}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b2c27b32-fdd2-4db9-b23b-7ec32a91d3be"/>
-    <ds:schemaRef ds:uri="650c6c8f-6c2a-41c5-9e0c-9cf06d8ec2d7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>